<commit_message>
Completed in first stage.using User and Development Table.Finished main business
</commit_message>
<xml_diff>
--- a/assert/templates/private0.xlsx
+++ b/assert/templates/private0.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -173,28 +173,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,67 +274,25 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>663120</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>349920</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="图片 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="378000" y="248400"/>
-          <a:ext cx="1451520" cy="589320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:I8"/>
+  <dimension ref="B4:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.79"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
@@ -340,12 +302,12 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -357,7 +319,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
@@ -383,6 +345,64 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D4:I4"/>
@@ -391,9 +411,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add excel's serial number
</commit_message>
<xml_diff>
--- a/assert/templates/private0.xlsx
+++ b/assert/templates/private0.xlsx
@@ -178,27 +178,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,6 +274,48 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>604440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>341640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="图像 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1188000" y="266400"/>
+          <a:ext cx="582840" cy="560880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -282,7 +324,7 @@
   <dimension ref="B4:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,5 +456,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
install pillow to support image copy
</commit_message>
<xml_diff>
--- a/assert/templates/private0.xlsx
+++ b/assert/templates/private0.xlsx
@@ -173,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,6 +187,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,9 +289,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>604440</xdr:colOff>
+      <xdr:colOff>604080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>341640</xdr:rowOff>
+      <xdr:rowOff>341280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -301,7 +305,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1188000" y="266400"/>
-          <a:ext cx="582840" cy="560880"/>
+          <a:ext cx="582480" cy="560520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,7 +328,7 @@
   <dimension ref="B4:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9:B18"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,47 +352,48 @@
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="6"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>